<commit_message>
modified:   solutions.xlsx: changed concentrations to new values
</commit_message>
<xml_diff>
--- a/calibrations/solutions.xlsx
+++ b/calibrations/solutions.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>fa</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>ph</t>
+  </si>
+  <si>
+    <t>density@50C</t>
+  </si>
+  <si>
+    <t>g/cc</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>ml</t>
   </si>
 </sst>
 </file>
@@ -111,9 +123,10 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -689,7 +702,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>100</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="8" ht="14.25">
@@ -701,7 +714,7 @@
       </c>
       <c r="C8">
         <f>C7*10^(-6)*1000/C5</f>
-        <v>0.0044382835101253607</v>
+        <v>4.4382835101253608</v>
       </c>
     </row>
     <row r="9" ht="14.25"/>
@@ -718,7 +731,7 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>160</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" ht="14.25">
@@ -741,7 +754,7 @@
       </c>
       <c r="C13">
         <f>C11*10^(-6)*C12*1000</f>
-        <v>17.295359999999999</v>
+        <v>11.890559999999999</v>
       </c>
     </row>
     <row r="14" ht="14.25"/>
@@ -758,7 +771,7 @@
         <v>9</v>
       </c>
       <c r="C16">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" ht="14.25">
@@ -781,7 +794,7 @@
       </c>
       <c r="C18">
         <f>C16*10^(-6)*C17*1000</f>
-        <v>15.415679999999998</v>
+        <v>14.314559999999998</v>
       </c>
     </row>
     <row r="19" ht="14.25"/>
@@ -798,7 +811,7 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <v>150</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" ht="14.25">
@@ -821,7 +834,7 @@
       </c>
       <c r="C23">
         <f>C21*10^(-6)*C22*1000</f>
-        <v>16.516799999999996</v>
+        <v>25.325759999999995</v>
       </c>
     </row>
     <row r="24" ht="14.25"/>
@@ -838,7 +851,7 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" ht="14.25">
@@ -861,10 +874,43 @@
       </c>
       <c r="C28">
         <f>C26*10^(-6)*C27*1000</f>
-        <v>16.940339999999999</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25"/>
+        <v>25.410510000000002</v>
+      </c>
+      <c r="D28" s="3">
+        <f>C28*10</f>
+        <v>254.10510000000002</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>1.0497000000000001</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1.0497000000000001</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30">
+        <f>C28*10^(-3)/C29</f>
+        <v>0.024207402114889972</v>
+      </c>
+      <c r="D30" s="2">
+        <f>D28*10^(-3)/D29</f>
+        <v>0.2420740211488997</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
added 'format' parameter to addexperiments command description
</commit_message>
<xml_diff>
--- a/calibrations/solutions.xlsx
+++ b/calibrations/solutions.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>fa</t>
   </si>
@@ -82,6 +82,21 @@
   </si>
   <si>
     <t>ml</t>
+  </si>
+  <si>
+    <t>H2O2</t>
+  </si>
+  <si>
+    <t>w.</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>g/ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc needed</t>
   </si>
 </sst>
 </file>
@@ -641,6 +656,7 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" min="1" max="1" width="14.421875"/>
+    <col bestFit="1" min="7" max="7" width="10.8515625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -910,6 +926,81 @@
         <v>0.89657044869962843</v>
       </c>
     </row>
+    <row r="32" ht="14.25">
+      <c r="A32" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>0.29999999999999999</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="2">
+        <v>34.014679999999998</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <f>C33*C34/C35*1000</f>
+        <v>9.7898907177724439</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25"/>
+    <row r="38" ht="14.25">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39">
+        <f>C38*10^(-6)/C36*1000</f>
+        <v>1.0214618618618618</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
changed concentration of h2o2 solution and do.cmd to see preliminary results of calibration
</commit_message>
<xml_diff>
--- a/calibrations/solutions.xlsx
+++ b/calibrations/solutions.xlsx
@@ -985,7 +985,7 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>10000</v>
+        <v>8500</v>
       </c>
     </row>
     <row r="39" ht="14.25">
@@ -997,10 +997,11 @@
       </c>
       <c r="C39">
         <f>C38*10^(-6)/C36*1000</f>
-        <v>1.0214618618618618</v>
+        <v>0.86824258258258247</v>
       </c>
     </row>
     <row r="40" ht="14.25"/>
+    <row r="41" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>